<commit_message>
Time Record Manager - Mid - 3rd March 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0038660_VerifyTheFunctionalityOfTimeRecordManagerForFVACAOUserOntheSFLightningView.xlsx
+++ b/TestData/LV_TMTT0038660_VerifyTheFunctionalityOfTimeRecordManagerForFVACAOUserOntheSFLightningView.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D4AF68-B427-4002-BF2F-033BCB0FC6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132CD1BC-03C7-4001-BB4F-C24C6D6E2868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -526,18 +526,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +548,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -562,7 +562,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -587,14 +587,14 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -612,17 +612,17 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -637,16 +637,16 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -657,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -668,7 +668,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
@@ -679,7 +679,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
     </row>
   </sheetData>
@@ -696,16 +696,16 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -716,7 +716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -727,7 +727,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -753,16 +753,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -782,7 +782,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -802,7 +802,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -823,21 +823,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -857,7 +857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -877,7 +877,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -902,14 +902,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -920,7 +920,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>41</v>
       </c>
@@ -931,7 +931,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>40</v>
       </c>

</xml_diff>